<commit_message>
Created Special Rules Table
</commit_message>
<xml_diff>
--- a/Special Rules Definition Document.xlsx
+++ b/Special Rules Definition Document.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23c70a194c994f0a/Documents/GitHub/Horus-Heresy-Game-Aid---Index-Cards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{E25ECAC3-207A-4FA4-976B-96187E2E2BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3032BE52-B50C-4E52-8D45-C48E321F50E0}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{E25ECAC3-207A-4FA4-976B-96187E2E2BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97712A28-2492-41E2-A588-10302DF4B4F9}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="2745" windowWidth="28800" windowHeight="11295" xr2:uid="{E0A51D4B-B1E0-48AD-AC96-F7985157B362}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{E0A51D4B-B1E0-48AD-AC96-F7985157B362}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t xml:space="preserve">Special Rule </t>
   </si>
@@ -234,10 +234,6 @@
     <t>Any models which suffer an unsaved wound or hull point loss from a weapon with this special rule instead suffer D6 unsaved Wounds of Hull Points of damage. _x000B_If the target of this attack is a Knight, Titan, Super-Heavy Vehicle, Building, Fortification or Monstrous unit type/subtype increase the number of wounds suffered or Hull points lost to 2D6</t>
   </si>
   <si>
-    <t>X denotes the number of attacks made when making a shooting attack with a Destroyer weapon. Models with Destroyer weapons may shoot and still charge in the Charge Phase. 
-In addition, when rolling for armour penetration with a Destroyer X weapon roll 3D6 and discard the lowest dice rolled, or any one of the lowest dice in the case of a tied result, Use the total of the remaining dice to determine the result</t>
-  </si>
-  <si>
     <t>Reactor Meltdown (Major)</t>
   </si>
   <si>
@@ -253,7 +249,7 @@
     <t>Reactor Meltdown (Maxima)</t>
   </si>
   <si>
-    <t xml:space="preserve">When a model with this Rule is destroyed, resolve hits caused by Catastrophic Damage as Destroyer Attacks at AP2 and double the range of the Catastrophic Damage effect. Refer to Destroyer Special rule. </t>
+    <t>X denotes the number of attacks made when making a shooting attack with a Destroyer weapon. Models with Destroyer weapons may shoot and still charge in the Charge Phase.  In addition, when rolling for armour penetration with a Destroyer X weapon roll 3D6 and discard the lowest dice rolled, or any one of the lowest dice in the case of a tied result, Use the total of the remaining dice to determine the result</t>
   </si>
 </sst>
 </file>
@@ -332,6 +328,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E079F0-EAAC-4362-83A2-46DCDFFA3452}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,7 +719,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -767,7 +767,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -775,7 +775,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -807,7 +807,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -823,7 +823,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -839,7 +839,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -855,7 +855,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
@@ -871,7 +871,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
@@ -919,37 +919,35 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="3" t="s">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>70</v>
-      </c>
+      <c r="B36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>